<commit_message>
*updated power converter design calculations
*added initial TINA simulation file
</commit_message>
<xml_diff>
--- a/DCDC/Calc/UCC2897A USB PD Forward Converter Annotated Deisgn Sheet.xlsx
+++ b/DCDC/Calc/UCC2897A USB PD Forward Converter Annotated Deisgn Sheet.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="167">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="213" uniqueCount="174">
   <si>
     <t>UCC2897A Controller Setup Tool</t>
   </si>
@@ -360,6 +360,15 @@
     <t>Δ IL/ (8 * Fsw *Vrpp )</t>
   </si>
   <si>
+    <t>Selected Output Capacitance</t>
+  </si>
+  <si>
+    <t>CO</t>
+  </si>
+  <si>
+    <t>uF</t>
+  </si>
+  <si>
     <t>Min Input Capacitance</t>
   </si>
   <si>
@@ -562,6 +571,18 @@
     <t>RIN2</t>
   </si>
   <si>
+    <t>RIN3(calculated)</t>
+  </si>
+  <si>
+    <t>RIN3(chosen)</t>
+  </si>
+  <si>
+    <t>RIN4(calculated)</t>
+  </si>
+  <si>
+    <t>RIN4(chosen)</t>
+  </si>
+  <si>
     <t>Current Sense Capacitor</t>
   </si>
   <si>
@@ -708,7 +729,7 @@
     </r>
   </si>
   <si>
-    <t>9*Rf*Fsw/(Dmax*dVL/dt)</t>
+    <t>2*5*Rf*Fsw/(Dmax*m*dVL/dt)</t>
   </si>
   <si>
     <t>Qg(main)</t>
@@ -1338,20 +1359,17 @@
     <xf borderId="2" fillId="3" fontId="6" numFmtId="1" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf borderId="2" fillId="4" fontId="6" numFmtId="2" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf borderId="12" fillId="4" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf borderId="20" fillId="4" fontId="6" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="3" fillId="4" fontId="6" numFmtId="2" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf borderId="2" fillId="2" fontId="6" numFmtId="2" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="2" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf borderId="2" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="2" fillId="3" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0"/>
+    </xf>
+    <xf borderId="2" fillId="4" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="left"/>
     </xf>
     <xf borderId="2" fillId="3" fontId="6" numFmtId="165" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
@@ -1369,6 +1387,9 @@
     <xf borderId="17" fillId="0" fontId="6" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="2" fillId="3" fontId="6" numFmtId="2" xfId="0" applyBorder="1" applyFont="1" applyNumberFormat="1"/>
     <xf borderId="2" fillId="4" fontId="6" numFmtId="2" xfId="0" applyBorder="1" applyFont="1" applyNumberFormat="1"/>
+    <xf borderId="12" fillId="4" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf borderId="3" fillId="4" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
@@ -2010,8 +2031,8 @@
         <v>47</v>
       </c>
       <c r="C31" s="7"/>
-      <c r="D31" s="21">
-        <v>0.1</v>
+      <c r="D31" s="24">
+        <v>0.2</v>
       </c>
       <c r="E31" s="22" t="s">
         <v>48</v>
@@ -2044,7 +2065,7 @@
         <v>51</v>
       </c>
       <c r="C34" s="7"/>
-      <c r="D34" s="21">
+      <c r="D34" s="24">
         <v>85.0</v>
       </c>
       <c r="E34" s="22" t="s">
@@ -2280,10 +2301,18 @@
     </row>
     <row r="45" ht="14.25" customHeight="1">
       <c r="A45" s="10"/>
-      <c r="B45" s="47"/>
-      <c r="C45" s="9"/>
-      <c r="D45" s="54"/>
-      <c r="E45" s="55"/>
+      <c r="B45" s="49" t="s">
+        <v>77</v>
+      </c>
+      <c r="C45" s="50" t="s">
+        <v>78</v>
+      </c>
+      <c r="D45" s="46">
+        <v>220.0</v>
+      </c>
+      <c r="E45" s="51" t="s">
+        <v>79</v>
+      </c>
       <c r="F45" s="10"/>
       <c r="G45" s="10"/>
       <c r="H45" s="10"/>
@@ -2308,606 +2337,646 @@
     </row>
     <row r="46" ht="14.25" customHeight="1">
       <c r="B46" s="47" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="C46" s="7" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="D46" s="48">
-        <f>1.25*1000000*(D22*D25+D78*0.01*D34*D10)*(1-D13)/(0.01*D34*D10*D29*1000*0.05*D10)</f>
+        <f>1.25*1000000*(D22*D25+D81*0.01*D34*D10)*(1-D13)/(0.01*D34*D10*D29*1000*0.05*D10)</f>
         <v>5.490264161</v>
       </c>
       <c r="E46" s="22" t="s">
         <v>73</v>
       </c>
       <c r="F46" s="45" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
     </row>
     <row r="47" ht="14.25" customHeight="1">
-      <c r="B47" s="56"/>
+      <c r="B47" s="54"/>
       <c r="C47" s="33"/>
-      <c r="D47" s="57"/>
+      <c r="D47" s="55"/>
       <c r="E47" s="39"/>
     </row>
     <row r="48" ht="14.25" customHeight="1">
       <c r="B48" s="23" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="C48" s="7" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="D48" s="48">
         <f>(D31-0.015)*1000/11.1</f>
-        <v>7.657657658</v>
+        <v>16.66666667</v>
       </c>
       <c r="E48" s="22" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="F48" s="45" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
     </row>
     <row r="49" ht="14.25" customHeight="1">
       <c r="B49" s="47" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="C49" s="7" t="s">
-        <v>85</v>
-      </c>
-      <c r="D49" s="58">
-        <v>8.45</v>
+        <v>88</v>
+      </c>
+      <c r="D49" s="46">
+        <v>20.0</v>
       </c>
       <c r="E49" s="22" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
     </row>
     <row r="50" ht="14.25" customHeight="1">
       <c r="B50" s="23" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
       <c r="C50" s="7" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="D50" s="48">
         <f>(I50+D31)*1000/36.1</f>
-        <v>65.09695291</v>
+        <v>67.86703601</v>
       </c>
       <c r="E50" s="22" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
       <c r="F50" s="45" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
       <c r="H50" s="2" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
       <c r="I50" s="2">
         <f>D13*1000/D29</f>
         <v>2.25</v>
       </c>
       <c r="J50" s="45" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
     </row>
     <row r="51" ht="14.25" customHeight="1">
       <c r="B51" s="47" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="C51" s="7" t="s">
-        <v>94</v>
-      </c>
-      <c r="D51" s="58">
-        <v>69.8</v>
+        <v>97</v>
+      </c>
+      <c r="D51" s="46">
+        <v>68.0</v>
       </c>
       <c r="E51" s="22" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
     </row>
     <row r="52" ht="14.25" customHeight="1">
       <c r="B52" s="23" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
       <c r="C52" s="7" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
       <c r="D52" s="48">
         <f>(I52-D31-0.17)*1000/15</f>
-        <v>165.3333333</v>
+        <v>158.6666667</v>
       </c>
       <c r="E52" s="22" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="F52" s="45" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="H52" s="2" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="I52" s="2">
         <f>(1-D13)*1000/D29</f>
         <v>2.75</v>
       </c>
       <c r="J52" s="45" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
     </row>
     <row r="53" ht="14.25" customHeight="1">
       <c r="B53" s="47" t="s">
-        <v>101</v>
+        <v>104</v>
       </c>
       <c r="C53" s="7" t="s">
-        <v>102</v>
+        <v>105</v>
       </c>
       <c r="D53" s="24">
         <v>160.0</v>
       </c>
       <c r="E53" s="22" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
     </row>
     <row r="54" ht="14.25" customHeight="1">
       <c r="B54" s="23" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
       <c r="C54" s="7" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="D54" s="53">
         <f>2.5*0.43*D30*0.001*1000000000/(D50*1000*2)</f>
-        <v>247.7074468</v>
+        <v>237.5969388</v>
       </c>
       <c r="E54" s="22" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="F54" s="45" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
     </row>
     <row r="55" ht="14.25" customHeight="1">
       <c r="B55" s="47" t="s">
-        <v>107</v>
+        <v>110</v>
       </c>
       <c r="C55" s="7" t="s">
+        <v>111</v>
+      </c>
+      <c r="D55" s="24">
+        <v>220.0</v>
+      </c>
+      <c r="E55" s="22" t="s">
         <v>108</v>
-      </c>
-      <c r="D55" s="21">
-        <v>220.0</v>
-      </c>
-      <c r="E55" s="22" t="s">
-        <v>105</v>
       </c>
     </row>
     <row r="56" ht="14.25" customHeight="1">
       <c r="B56" s="23"/>
       <c r="C56" s="7"/>
-      <c r="D56" s="59"/>
+      <c r="D56" s="56"/>
       <c r="E56" s="22"/>
       <c r="H56" s="2" t="s">
-        <v>109</v>
+        <v>112</v>
       </c>
       <c r="I56" s="2">
         <f>2.5*0.05/(D49*1000)</f>
-        <v>0.00001479289941</v>
+        <v>0.00000625</v>
       </c>
     </row>
     <row r="57" ht="14.25" customHeight="1">
       <c r="B57" s="23" t="s">
-        <v>110</v>
+        <v>113</v>
       </c>
       <c r="C57" s="7" t="s">
-        <v>111</v>
+        <v>114</v>
       </c>
       <c r="D57" s="26">
         <f>(D17-D18)*0.001/I56</f>
-        <v>67.6</v>
+        <v>160</v>
       </c>
       <c r="E57" s="22" t="s">
-        <v>112</v>
+        <v>115</v>
       </c>
     </row>
     <row r="58" ht="14.25" customHeight="1">
       <c r="B58" s="23" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="C58" s="7" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
       <c r="D58" s="24">
-        <v>400.0</v>
+        <v>160.0</v>
       </c>
       <c r="E58" s="22" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
     </row>
     <row r="59" ht="14.25" customHeight="1">
       <c r="B59" s="23" t="s">
-        <v>115</v>
+        <v>118</v>
       </c>
       <c r="C59" s="7" t="s">
-        <v>116</v>
+        <v>119</v>
       </c>
       <c r="D59" s="48">
         <f>D57*1.27/(34.6-1.27)</f>
-        <v>2.575817582</v>
+        <v>6.096609661</v>
       </c>
       <c r="E59" s="22" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
     </row>
     <row r="60" ht="14.25" customHeight="1">
       <c r="B60" s="23" t="s">
-        <v>117</v>
+        <v>120</v>
       </c>
       <c r="C60" s="7" t="s">
-        <v>118</v>
+        <v>121</v>
       </c>
       <c r="D60" s="24">
-        <v>16.0</v>
+        <v>6.2</v>
       </c>
       <c r="E60" s="22" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
     </row>
     <row r="61" ht="14.25" customHeight="1">
-      <c r="B61" s="23"/>
+      <c r="B61" s="20" t="s">
+        <v>122</v>
+      </c>
       <c r="C61" s="7"/>
-      <c r="D61" s="59"/>
+      <c r="D61" s="57">
+        <f>(D16-D12)*0.001/I56</f>
+        <v>480</v>
+      </c>
       <c r="E61" s="22"/>
     </row>
     <row r="62" ht="14.25" customHeight="1">
-      <c r="B62" s="23"/>
+      <c r="B62" s="20" t="s">
+        <v>123</v>
+      </c>
       <c r="C62" s="7"/>
-      <c r="D62" s="59"/>
-      <c r="E62" s="22"/>
+      <c r="D62" s="24">
+        <v>470.0</v>
+      </c>
+      <c r="E62" s="25" t="s">
+        <v>89</v>
+      </c>
     </row>
     <row r="63" ht="14.25" customHeight="1">
-      <c r="B63" s="47" t="s">
-        <v>119</v>
-      </c>
-      <c r="C63" s="7" t="s">
-        <v>120</v>
-      </c>
-      <c r="D63" s="21">
+      <c r="B63" s="20" t="s">
+        <v>124</v>
+      </c>
+      <c r="C63" s="7"/>
+      <c r="D63" s="26">
+        <f>D61*1.27/(34.6-1.27)</f>
+        <v>18.28982898</v>
+      </c>
+      <c r="E63" s="25" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="64" ht="14.25" customHeight="1">
+      <c r="B64" s="20" t="s">
+        <v>125</v>
+      </c>
+      <c r="C64" s="7"/>
+      <c r="D64" s="21">
+        <f>18</f>
+        <v>18</v>
+      </c>
+      <c r="E64" s="25" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="65" ht="14.25" customHeight="1">
+      <c r="B65" s="20"/>
+      <c r="C65" s="7"/>
+      <c r="D65" s="58"/>
+      <c r="E65" s="25"/>
+    </row>
+    <row r="66" ht="14.25" customHeight="1">
+      <c r="B66" s="47" t="s">
+        <v>126</v>
+      </c>
+      <c r="C66" s="7" t="s">
+        <v>127</v>
+      </c>
+      <c r="D66" s="21">
         <v>100.0</v>
       </c>
-      <c r="E63" s="22" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="64" ht="14.25" customHeight="1">
-      <c r="B64" s="23" t="s">
-        <v>122</v>
-      </c>
-      <c r="C64" s="7" t="s">
-        <v>123</v>
-      </c>
-      <c r="D64" s="53">
-        <f>1/(2*3.14*D29*10000*D63*1E-12)</f>
-        <v>796.1783439</v>
-      </c>
-      <c r="E64" s="22" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="65" ht="14.25" customHeight="1">
-      <c r="B65" s="47" t="s">
-        <v>125</v>
-      </c>
-      <c r="C65" s="7" t="s">
-        <v>126</v>
-      </c>
-      <c r="D65" s="21">
-        <v>680.0</v>
-      </c>
-      <c r="E65" s="22" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="66" ht="14.25" customHeight="1">
-      <c r="B66" s="23"/>
-      <c r="C66" s="7"/>
-      <c r="D66" s="59"/>
-      <c r="E66" s="22"/>
+      <c r="E66" s="22" t="s">
+        <v>128</v>
+      </c>
     </row>
     <row r="67" ht="14.25" customHeight="1">
       <c r="B67" s="23" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="C67" s="7" t="s">
-        <v>128</v>
-      </c>
-      <c r="D67" s="60">
-        <f>0.43/I67</f>
+        <v>130</v>
+      </c>
+      <c r="D67" s="53">
+        <f>1/(2*3.14*D29*10000*D66*1E-12)</f>
+        <v>796.1783439</v>
+      </c>
+      <c r="E67" s="22" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="68" ht="14.25" customHeight="1">
+      <c r="B68" s="47" t="s">
+        <v>132</v>
+      </c>
+      <c r="C68" s="7" t="s">
+        <v>133</v>
+      </c>
+      <c r="D68" s="24">
+        <v>820.0</v>
+      </c>
+      <c r="E68" s="22" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="69" ht="14.25" customHeight="1">
+      <c r="B69" s="23"/>
+      <c r="C69" s="7"/>
+      <c r="D69" s="56"/>
+      <c r="E69" s="22"/>
+    </row>
+    <row r="70" ht="14.25" customHeight="1">
+      <c r="B70" s="23" t="s">
+        <v>134</v>
+      </c>
+      <c r="C70" s="7" t="s">
+        <v>135</v>
+      </c>
+      <c r="D70" s="59">
+        <f>0.43/I70</f>
         <v>0.1171370534</v>
       </c>
-      <c r="E67" s="22" t="s">
-        <v>124</v>
-      </c>
-      <c r="F67" s="45" t="s">
-        <v>129</v>
-      </c>
-      <c r="H67" s="2" t="s">
-        <v>130</v>
-      </c>
-      <c r="I67" s="61">
-        <f>(D26+D26*D15/100)/D72</f>
+      <c r="E70" s="22" t="s">
+        <v>131</v>
+      </c>
+      <c r="F70" s="45" t="s">
+        <v>136</v>
+      </c>
+      <c r="H70" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="I70" s="60">
+        <f>(D26+D26*D15/100)/D75</f>
         <v>3.67091358</v>
       </c>
     </row>
-    <row r="68" ht="14.25" customHeight="1">
-      <c r="B68" s="62"/>
-      <c r="C68" s="63"/>
-      <c r="D68" s="64"/>
-      <c r="E68" s="31"/>
-    </row>
-    <row r="69" ht="14.25" customHeight="1">
-      <c r="B69" s="37"/>
-      <c r="C69" s="33"/>
-      <c r="D69" s="38"/>
-      <c r="E69" s="39"/>
-    </row>
-    <row r="70" ht="14.25" customHeight="1">
-      <c r="B70" s="37"/>
-      <c r="C70" s="33"/>
-      <c r="D70" s="38"/>
-      <c r="E70" s="39"/>
-    </row>
     <row r="71" ht="14.25" customHeight="1">
-      <c r="B71" s="23" t="s">
-        <v>131</v>
-      </c>
-      <c r="C71" s="7" t="s">
-        <v>132</v>
-      </c>
-      <c r="D71" s="65">
+      <c r="B71" s="61"/>
+      <c r="C71" s="62"/>
+      <c r="D71" s="63"/>
+      <c r="E71" s="31"/>
+    </row>
+    <row r="72" ht="14.25" customHeight="1">
+      <c r="B72" s="37"/>
+      <c r="C72" s="33"/>
+      <c r="D72" s="38"/>
+      <c r="E72" s="39"/>
+    </row>
+    <row r="73" ht="14.25" customHeight="1">
+      <c r="B73" s="37"/>
+      <c r="C73" s="33"/>
+      <c r="D73" s="38"/>
+      <c r="E73" s="39"/>
+    </row>
+    <row r="74" ht="14.25" customHeight="1">
+      <c r="B74" s="23" t="s">
+        <v>138</v>
+      </c>
+      <c r="C74" s="7" t="s">
+        <v>139</v>
+      </c>
+      <c r="D74" s="64">
         <f>(D22+0.2)/D13</f>
         <v>44.88888889</v>
       </c>
-      <c r="E71" s="22"/>
-      <c r="F71" s="45" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="72" ht="14.25" customHeight="1">
-      <c r="B72" s="23" t="s">
-        <v>134</v>
-      </c>
-      <c r="C72" s="52" t="s">
-        <v>135</v>
-      </c>
-      <c r="D72" s="48">
-        <f>D10/D71</f>
-        <v>1.002475248</v>
-      </c>
-      <c r="E72" s="22"/>
-      <c r="F72" s="45" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="73" ht="14.25" customHeight="1">
-      <c r="B73" s="23"/>
-      <c r="C73" s="7"/>
-      <c r="D73" s="59"/>
-      <c r="E73" s="22"/>
-      <c r="H73" s="2" t="s">
-        <v>137</v>
-      </c>
-      <c r="I73" s="2">
-        <f>(D10-D22*D72)*100*D67/(D72^2*D37*D33)</f>
-        <v>2.143375556</v>
-      </c>
-      <c r="J73" s="45" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="74" ht="14.25" customHeight="1">
-      <c r="B74" s="23"/>
-      <c r="C74" s="7"/>
-      <c r="D74" s="59"/>
       <c r="E74" s="22"/>
-      <c r="H74" s="2" t="s">
-        <v>3</v>
+      <c r="F74" s="45" t="s">
+        <v>140</v>
       </c>
     </row>
     <row r="75" ht="14.25" customHeight="1">
       <c r="B75" s="23" t="s">
-        <v>139</v>
-      </c>
-      <c r="C75" s="7" t="s">
-        <v>140</v>
-      </c>
-      <c r="D75" s="53">
-        <f>9*D65*D29*0.001/(D13*I73*1000)</f>
-        <v>1.269026323</v>
-      </c>
-      <c r="E75" s="22" t="s">
-        <v>86</v>
-      </c>
+        <v>141</v>
+      </c>
+      <c r="C75" s="52" t="s">
+        <v>142</v>
+      </c>
+      <c r="D75" s="48">
+        <f>D10/D74</f>
+        <v>1.002475248</v>
+      </c>
+      <c r="E75" s="22"/>
       <c r="F75" s="45" t="s">
-        <v>141</v>
-      </c>
-      <c r="H75" s="45" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
     </row>
     <row r="76" ht="14.25" customHeight="1">
-      <c r="B76" s="37"/>
-      <c r="C76" s="33"/>
-      <c r="D76" s="33"/>
-      <c r="E76" s="66"/>
-      <c r="H76" s="45" t="s">
-        <v>143</v>
+      <c r="B76" s="23"/>
+      <c r="C76" s="7"/>
+      <c r="D76" s="56"/>
+      <c r="E76" s="22"/>
+      <c r="H76" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="I76" s="2">
+        <f>(D10-D22*D75)*100*D70/(D75^2*D37*D33)</f>
+        <v>2.143375556</v>
+      </c>
+      <c r="J76" s="45" t="s">
+        <v>145</v>
       </c>
     </row>
     <row r="77" ht="14.25" customHeight="1">
-      <c r="B77" s="37"/>
-      <c r="C77" s="33"/>
-      <c r="D77" s="33"/>
-      <c r="E77" s="66"/>
-      <c r="H77" s="45" t="s">
-        <v>144</v>
-      </c>
-      <c r="I77" s="2">
-        <f>(I75+I76)/0.1</f>
+      <c r="B77" s="23"/>
+      <c r="C77" s="7"/>
+      <c r="D77" s="56"/>
+      <c r="E77" s="22"/>
+      <c r="H77" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="78" ht="14.25" customHeight="1">
+      <c r="B78" s="23" t="s">
+        <v>146</v>
+      </c>
+      <c r="C78" s="7" t="s">
+        <v>147</v>
+      </c>
+      <c r="D78" s="53">
+        <f>9*D68*D29*0.001/(D13*I76*1000)</f>
+        <v>1.530296448</v>
+      </c>
+      <c r="E78" s="22" t="s">
+        <v>89</v>
+      </c>
+      <c r="F78" s="45" t="s">
+        <v>148</v>
+      </c>
+      <c r="H78" s="45" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="79" ht="14.25" customHeight="1">
+      <c r="B79" s="37"/>
+      <c r="C79" s="33"/>
+      <c r="D79" s="33"/>
+      <c r="E79" s="65"/>
+      <c r="H79" s="45" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="80" ht="14.25" customHeight="1">
+      <c r="B80" s="37"/>
+      <c r="C80" s="33"/>
+      <c r="D80" s="33"/>
+      <c r="E80" s="65"/>
+      <c r="H80" s="45" t="s">
+        <v>151</v>
+      </c>
+      <c r="I80" s="2">
+        <f>(I78+I79)/0.1</f>
         <v>0</v>
       </c>
     </row>
-    <row r="78" ht="14.25" customHeight="1">
-      <c r="B78" s="47" t="s">
-        <v>145</v>
-      </c>
-      <c r="C78" s="7" t="s">
-        <v>146</v>
-      </c>
-      <c r="D78" s="67">
+    <row r="81" ht="14.25" customHeight="1">
+      <c r="B81" s="47" t="s">
+        <v>152</v>
+      </c>
+      <c r="C81" s="7" t="s">
+        <v>153</v>
+      </c>
+      <c r="D81" s="66">
         <f>D10*D13/(D29*D19*0.001)</f>
         <v>2.025</v>
       </c>
-      <c r="E78" s="22" t="s">
+      <c r="E81" s="22" t="s">
         <v>39</v>
       </c>
-      <c r="F78" s="45" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="79" ht="14.25" customHeight="1">
-      <c r="B79" s="47" t="s">
-        <v>148</v>
-      </c>
-      <c r="C79" s="7" t="s">
-        <v>149</v>
-      </c>
-      <c r="D79" s="67">
-        <f>D78+D40/D72</f>
-        <v>5.186778516</v>
-      </c>
-      <c r="E79" s="22" t="s">
-        <v>39</v>
-      </c>
-      <c r="F79" s="45" t="s">
-        <v>150</v>
-      </c>
-      <c r="H79" s="45" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="80" ht="14.25" customHeight="1">
-      <c r="B80" s="49" t="s">
-        <v>152</v>
-      </c>
-      <c r="C80" s="7" t="s">
-        <v>153</v>
-      </c>
-      <c r="D80" s="67">
-        <f>(D41/D72)+D78/2</f>
-        <v>3.01999214</v>
-      </c>
-      <c r="E80" s="22" t="s">
-        <v>39</v>
-      </c>
-      <c r="F80" s="45" t="s">
+      <c r="F81" s="45" t="s">
         <v>154</v>
       </c>
-      <c r="H80" s="45" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="81" ht="14.25" customHeight="1">
-      <c r="A81" s="10"/>
-      <c r="B81" s="47"/>
-      <c r="C81" s="9"/>
-      <c r="D81" s="68"/>
-      <c r="E81" s="55"/>
-      <c r="F81" s="10"/>
-      <c r="G81" s="10"/>
-      <c r="H81" s="69" t="s">
-        <v>156</v>
-      </c>
-      <c r="I81" s="10"/>
-      <c r="J81" s="10"/>
-      <c r="K81" s="10"/>
-      <c r="L81" s="10"/>
-      <c r="M81" s="10"/>
-      <c r="N81" s="10"/>
-      <c r="O81" s="10"/>
-      <c r="P81" s="10"/>
-      <c r="Q81" s="10"/>
-      <c r="R81" s="10"/>
-      <c r="S81" s="10"/>
-      <c r="T81" s="10"/>
-      <c r="U81" s="10"/>
-      <c r="V81" s="10"/>
-      <c r="W81" s="10"/>
-      <c r="X81" s="10"/>
-      <c r="Y81" s="10"/>
-      <c r="Z81" s="10"/>
     </row>
     <row r="82" ht="14.25" customHeight="1">
       <c r="B82" s="47" t="s">
+        <v>155</v>
+      </c>
+      <c r="C82" s="7" t="s">
+        <v>156</v>
+      </c>
+      <c r="D82" s="66">
+        <f>D81+D40/D75</f>
+        <v>5.186778516</v>
+      </c>
+      <c r="E82" s="22" t="s">
+        <v>39</v>
+      </c>
+      <c r="F82" s="45" t="s">
         <v>157</v>
       </c>
-      <c r="C82" s="7" t="s">
+      <c r="H82" s="45" t="s">
         <v>158</v>
       </c>
-      <c r="D82" s="70">
+    </row>
+    <row r="83" ht="14.25" customHeight="1">
+      <c r="B83" s="49" t="s">
+        <v>159</v>
+      </c>
+      <c r="C83" s="7" t="s">
+        <v>160</v>
+      </c>
+      <c r="D83" s="66">
+        <f>(D41/D75)+D81/2</f>
+        <v>3.01999214</v>
+      </c>
+      <c r="E83" s="22" t="s">
+        <v>39</v>
+      </c>
+      <c r="F83" s="45" t="s">
+        <v>161</v>
+      </c>
+      <c r="H83" s="45" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="84" ht="14.25" customHeight="1">
+      <c r="A84" s="10"/>
+      <c r="B84" s="47"/>
+      <c r="C84" s="9"/>
+      <c r="D84" s="67"/>
+      <c r="E84" s="68"/>
+      <c r="F84" s="10"/>
+      <c r="G84" s="10"/>
+      <c r="H84" s="69" t="s">
+        <v>163</v>
+      </c>
+      <c r="I84" s="10"/>
+      <c r="J84" s="10"/>
+      <c r="K84" s="10"/>
+      <c r="L84" s="10"/>
+      <c r="M84" s="10"/>
+      <c r="N84" s="10"/>
+      <c r="O84" s="10"/>
+      <c r="P84" s="10"/>
+      <c r="Q84" s="10"/>
+      <c r="R84" s="10"/>
+      <c r="S84" s="10"/>
+      <c r="T84" s="10"/>
+      <c r="U84" s="10"/>
+      <c r="V84" s="10"/>
+      <c r="W84" s="10"/>
+      <c r="X84" s="10"/>
+      <c r="Y84" s="10"/>
+      <c r="Z84" s="10"/>
+    </row>
+    <row r="85" ht="14.25" customHeight="1">
+      <c r="B85" s="47" t="s">
+        <v>164</v>
+      </c>
+      <c r="C85" s="7" t="s">
+        <v>165</v>
+      </c>
+      <c r="D85" s="70">
         <f>D12/(1-D14)</f>
         <v>85.16535433</v>
       </c>
-      <c r="E82" s="22" t="s">
+      <c r="E85" s="22" t="s">
         <v>12</v>
       </c>
-      <c r="F82" s="45" t="s">
-        <v>159</v>
-      </c>
-      <c r="H82" s="45" t="s">
-        <v>160</v>
-      </c>
-      <c r="I82" s="2">
-        <f>(I80+I81+(I75+I76)*D29)*I80</f>
+      <c r="F85" s="45" t="s">
+        <v>166</v>
+      </c>
+      <c r="H85" s="45" t="s">
+        <v>167</v>
+      </c>
+      <c r="I85" s="2">
+        <f>(I83+I84+(I78+I79)*D29)*I83</f>
         <v>0</v>
       </c>
     </row>
-    <row r="83" ht="14.25" customHeight="1">
-      <c r="B83" s="37"/>
-      <c r="C83" s="33"/>
-      <c r="D83" s="33"/>
-      <c r="E83" s="66"/>
-      <c r="H83" s="45" t="s">
-        <v>161</v>
-      </c>
-      <c r="I83" s="45">
-        <f>2*I82*D30*0.001/(12.7^2-8^2)</f>
+    <row r="86" ht="14.25" customHeight="1">
+      <c r="B86" s="37"/>
+      <c r="C86" s="33"/>
+      <c r="D86" s="33"/>
+      <c r="E86" s="65"/>
+      <c r="H86" s="45" t="s">
+        <v>168</v>
+      </c>
+      <c r="I86" s="45">
+        <f>2*I85*D30*0.001/(12.7^2-8^2)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="84" ht="14.25" customHeight="1">
-      <c r="B84" s="37"/>
-      <c r="C84" s="33"/>
-      <c r="D84" s="33"/>
-      <c r="E84" s="66"/>
-    </row>
-    <row r="85" ht="14.25" customHeight="1">
-      <c r="B85" s="71" t="s">
-        <v>162</v>
-      </c>
-      <c r="C85" s="72" t="s">
-        <v>163</v>
-      </c>
-      <c r="D85" s="73">
+    <row r="87" ht="14.25" customHeight="1">
+      <c r="B87" s="37"/>
+      <c r="C87" s="33"/>
+      <c r="D87" s="33"/>
+      <c r="E87" s="65"/>
+    </row>
+    <row r="88" ht="14.25" customHeight="1">
+      <c r="B88" s="71" t="s">
+        <v>169</v>
+      </c>
+      <c r="C88" s="72" t="s">
+        <v>170</v>
+      </c>
+      <c r="D88" s="73">
         <f>1000000000*10*(1-D14)^2/((D19*0.000001)*(2*3.14159*D29*1000)^2)</f>
         <v>47.21628062</v>
       </c>
-      <c r="E85" s="74" t="s">
-        <v>105</v>
-      </c>
-      <c r="F85" s="45" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="86" ht="14.25" customHeight="1"/>
-    <row r="87" ht="14.25" customHeight="1"/>
-    <row r="88" ht="14.25" customHeight="1"/>
+      <c r="E88" s="74" t="s">
+        <v>108</v>
+      </c>
+      <c r="F88" s="45" t="s">
+        <v>171</v>
+      </c>
+    </row>
     <row r="89" ht="14.25" customHeight="1"/>
     <row r="90" ht="14.25" customHeight="1"/>
     <row r="91" ht="14.25" customHeight="1"/>
@@ -3821,6 +3890,9 @@
     <row r="999" ht="14.25" customHeight="1"/>
     <row r="1000" ht="14.25" customHeight="1"/>
     <row r="1001" ht="14.25" customHeight="1"/>
+    <row r="1002" ht="14.25" customHeight="1"/>
+    <row r="1003" ht="14.25" customHeight="1"/>
+    <row r="1004" ht="14.25" customHeight="1"/>
   </sheetData>
   <mergeCells count="7">
     <mergeCell ref="B1:E1"/>
@@ -3873,7 +3945,7 @@
     <row r="20" ht="14.25" customHeight="1"/>
     <row r="21" ht="14.25" customHeight="1">
       <c r="L21" s="6" t="s">
-        <v>165</v>
+        <v>172</v>
       </c>
     </row>
     <row r="22" ht="14.25" customHeight="1"/>
@@ -3889,7 +3961,7 @@
     <row r="32" ht="14.25" customHeight="1"/>
     <row r="33" ht="14.25" customHeight="1">
       <c r="C33" s="6" t="s">
-        <v>166</v>
+        <v>173</v>
       </c>
     </row>
     <row r="34" ht="14.25" customHeight="1"/>

</xml_diff>